<commit_message>
push to git by dinh
</commit_message>
<xml_diff>
--- a/excel/write-excel/new.xlsx
+++ b/excel/write-excel/new.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>stt</t>
   </si>
@@ -24,15 +24,6 @@
   </si>
   <si>
     <t>ngaysinh</t>
-  </si>
-  <si>
-    <t>Nguyen Van Dinh1</t>
-  </si>
-  <si>
-    <t>Nguyen Van Dinh2</t>
-  </si>
-  <si>
-    <t>Nguyen Van Dinh3</t>
   </si>
   <si>
     <t>tuoi</t>
@@ -72,7 +63,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -117,23 +108,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C3" sqref="C3"/>
@@ -439,39 +422,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1991</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1992</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1993</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -479,7 +429,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C1" sqref="C1"/>
@@ -495,7 +445,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>